<commit_message>
New functions in indexPanel
Plots for indexes in indexPanel added. New Excel file for testing created. indeksy.py updated for new exceptions.
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Animal 1</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>tekst</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>year 2011</t>
+  </si>
+  <si>
+    <t>year 2012</t>
+  </si>
+  <si>
+    <t>year 2013</t>
+  </si>
+  <si>
+    <t>year 2014</t>
+  </si>
+  <si>
+    <t>year 2015</t>
   </si>
 </sst>
 </file>
@@ -380,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -393,33 +411,36 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
+      <c r="F1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>26</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
       <c r="E2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -427,16 +448,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
+      <c r="E3">
         <v>3</v>
-      </c>
-      <c r="E3">
-        <v>56</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -444,16 +465,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
       <c r="E4">
-        <v>456</v>
+        <v>56</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -461,16 +482,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>16</v>
       </c>
       <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>456</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -478,16 +499,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>324</v>
+      <c r="E6" t="s">
+        <v>10</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -495,16 +516,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
       <c r="E7">
-        <v>23</v>
+        <v>324</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -512,16 +533,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
       <c r="E8">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -529,32 +550,49 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>33</v>
-      </c>
       <c r="E9">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>54</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>43</v>
       </c>
       <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>43</v>
+      </c>
+      <c r="F11">
         <v>1</v>
       </c>
     </row>

</xml_diff>